<commit_message>
Added the readme for the application
</commit_message>
<xml_diff>
--- a/doc/BikeRide-Model.xlsx
+++ b/doc/BikeRide-Model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fehac2\Downloads\Personal\BikeRide\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fehac2\IdeaProjects\bikeride-lagom\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -473,9 +473,6 @@
     <t>rideParticipants</t>
   </si>
   <si>
-    <t>members</t>
-  </si>
-  <si>
     <t>leaders</t>
   </si>
   <si>
@@ -639,6 +636,9 @@
   </si>
   <si>
     <t>SearchBikers</t>
+  </si>
+  <si>
+    <t>participants</t>
   </si>
 </sst>
 </file>
@@ -1228,46 +1228,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1278,133 +1242,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1414,15 +1276,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1432,8 +1285,155 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1743,25 +1743,25 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B5" s="1"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B8" s="1"/>
     </row>
@@ -1823,7 +1823,7 @@
   <dimension ref="B1:S52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4:N11"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -1849,91 +1849,91 @@
   <sheetData>
     <row r="1" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
-      <c r="Q2" s="42"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="43"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="47"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="49"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="19" t="s">
+      <c r="E3" s="73"/>
+      <c r="F3" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="20" t="s">
+      <c r="H3" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="N3" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q3" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="I3" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="J3" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="K3" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="L3" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="N3" s="81" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="P3" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q3" s="61" t="s">
-        <v>164</v>
-      </c>
-      <c r="R3" s="62"/>
-      <c r="S3" s="63"/>
+      <c r="R3" s="61"/>
+      <c r="S3" s="62"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="22" t="s">
+      <c r="E4" s="74"/>
+      <c r="F4" s="10" t="s">
         <v>74</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -1943,241 +1943,241 @@
       <c r="I4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="36" t="s">
+      <c r="J4" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="10" t="s">
         <v>96</v>
       </c>
       <c r="L4" s="1"/>
-      <c r="M4" s="23" t="s">
+      <c r="M4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="28" t="s">
+      <c r="O4" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="P4" s="30" t="s">
+      <c r="P4" s="84" t="s">
         <v>106</v>
       </c>
-      <c r="Q4" s="64"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="66"/>
+      <c r="Q4" s="51"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="53"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="17"/>
-      <c r="F5" s="22" t="s">
+      <c r="E5" s="74"/>
+      <c r="F5" s="10" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="K5" s="10" t="s">
         <v>96</v>
       </c>
       <c r="L5" s="1"/>
-      <c r="M5" s="23" t="s">
+      <c r="M5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="46" t="s">
+      <c r="N5" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="O5" s="28"/>
-      <c r="P5" s="30"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="68"/>
-      <c r="S5" s="69"/>
+      <c r="O5" s="44"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="56"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B6" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="23" t="s">
+      <c r="B6" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="22" t="s">
+      <c r="E6" s="74"/>
+      <c r="F6" s="10" t="s">
         <v>76</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J6" s="37" t="s">
+      <c r="J6" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="10" t="s">
         <v>96</v>
       </c>
       <c r="L6" s="1"/>
-      <c r="M6" s="23" t="s">
+      <c r="M6" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="N6" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="N6" s="46" t="s">
-        <v>202</v>
-      </c>
-      <c r="O6" s="28"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="67"/>
-      <c r="R6" s="68"/>
-      <c r="S6" s="69"/>
+      <c r="O6" s="44"/>
+      <c r="P6" s="84"/>
+      <c r="Q6" s="54"/>
+      <c r="R6" s="55"/>
+      <c r="S6" s="56"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="23" t="s">
+      <c r="C7" s="44"/>
+      <c r="D7" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="22" t="s">
+      <c r="E7" s="74"/>
+      <c r="F7" s="10" t="s">
         <v>76</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J7" s="37" t="s">
+      <c r="J7" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="10" t="s">
         <v>96</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="N7" s="46" t="s">
+      <c r="N7" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="28"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="68"/>
-      <c r="S7" s="69"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="84"/>
+      <c r="Q7" s="54"/>
+      <c r="R7" s="55"/>
+      <c r="S7" s="56"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="28"/>
-      <c r="D8" s="23" t="s">
+      <c r="C8" s="44"/>
+      <c r="D8" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="17"/>
-      <c r="F8" s="22" t="s">
+      <c r="E8" s="74"/>
+      <c r="F8" s="10" t="s">
         <v>76</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J8" s="37" t="s">
+      <c r="J8" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K8" s="22" t="s">
+      <c r="K8" s="10" t="s">
         <v>96</v>
       </c>
       <c r="L8" s="1"/>
-      <c r="M8" s="23" t="s">
+      <c r="M8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="46" t="s">
+      <c r="N8" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="O8" s="28"/>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="67"/>
-      <c r="R8" s="68"/>
-      <c r="S8" s="69"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="84"/>
+      <c r="Q8" s="54"/>
+      <c r="R8" s="55"/>
+      <c r="S8" s="56"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="23" t="s">
+      <c r="C9" s="44"/>
+      <c r="D9" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="22" t="s">
+      <c r="E9" s="74"/>
+      <c r="F9" s="10" t="s">
         <v>76</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I9" s="16" t="s">
+      <c r="I9" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J9" s="37" t="s">
+      <c r="J9" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="10" t="s">
         <v>96</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="M9" s="23" t="s">
+      <c r="M9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="N9" s="46" t="s">
+      <c r="N9" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="O9" s="28"/>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="67"/>
-      <c r="R9" s="68"/>
-      <c r="S9" s="69"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="84"/>
+      <c r="Q9" s="54"/>
+      <c r="R9" s="55"/>
+      <c r="S9" s="56"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="23" t="s">
+      <c r="C10" s="44"/>
+      <c r="D10" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="17"/>
-      <c r="F10" s="22" t="s">
+      <c r="E10" s="74"/>
+      <c r="F10" s="10" t="s">
         <v>74</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -2187,37 +2187,37 @@
         <v>109</v>
       </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="36" t="s">
+      <c r="J10" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="K10" s="22" t="s">
+      <c r="K10" s="10" t="s">
         <v>96</v>
       </c>
       <c r="L10" s="1"/>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="N10" s="18" t="s">
+      <c r="N10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O10" s="28"/>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="68"/>
-      <c r="S10" s="69"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="55"/>
+      <c r="S10" s="56"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="22" t="s">
+      <c r="E11" s="74"/>
+      <c r="F11" s="10" t="s">
         <v>74</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -2227,111 +2227,111 @@
         <v>109</v>
       </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="36" t="s">
+      <c r="J11" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="K11" s="10" t="s">
         <v>96</v>
       </c>
       <c r="L11" s="1"/>
-      <c r="M11" s="23" t="s">
+      <c r="M11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="N11" s="18" t="s">
+      <c r="N11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="O11" s="28"/>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="67"/>
-      <c r="R11" s="68"/>
-      <c r="S11" s="69"/>
+      <c r="O11" s="44"/>
+      <c r="P11" s="84"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="55"/>
+      <c r="S11" s="56"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="23" t="s">
+      <c r="C12" s="76"/>
+      <c r="D12" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="22" t="s">
+      <c r="E12" s="74"/>
+      <c r="F12" s="10" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>109</v>
       </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="36" t="s">
+      <c r="J12" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="10" t="s">
         <v>98</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="M12" s="23"/>
-      <c r="N12" s="82"/>
-      <c r="O12" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="M12" s="11"/>
+      <c r="N12" s="79"/>
+      <c r="O12" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="67"/>
-      <c r="R12" s="68"/>
-      <c r="S12" s="69"/>
+      <c r="P12" s="84"/>
+      <c r="Q12" s="54"/>
+      <c r="R12" s="55"/>
+      <c r="S12" s="56"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="D13" s="23" t="s">
+      <c r="C13" s="77" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="22" t="s">
+      <c r="E13" s="74"/>
+      <c r="F13" s="10" t="s">
         <v>85</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>109</v>
       </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="36" t="s">
+      <c r="J13" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="K13" s="22" t="s">
+      <c r="K13" s="10" t="s">
         <v>98</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="M13" s="23"/>
-      <c r="N13" s="83"/>
-      <c r="O13" s="5"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="67"/>
-      <c r="R13" s="68"/>
-      <c r="S13" s="69"/>
+        <v>198</v>
+      </c>
+      <c r="M13" s="11"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="82"/>
+      <c r="P13" s="84"/>
+      <c r="Q13" s="54"/>
+      <c r="R13" s="55"/>
+      <c r="S13" s="56"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="23" t="s">
+      <c r="C14" s="78"/>
+      <c r="D14" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="22" t="s">
+      <c r="E14" s="74"/>
+      <c r="F14" s="10" t="s">
         <v>85</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -2341,29 +2341,29 @@
         <v>109</v>
       </c>
       <c r="I14" s="1"/>
-      <c r="J14" s="36" t="s">
+      <c r="J14" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="22" t="s">
+      <c r="K14" s="10" t="s">
         <v>98</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="23"/>
-      <c r="N14" s="83"/>
-      <c r="O14" s="5"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="67"/>
-      <c r="R14" s="68"/>
-      <c r="S14" s="69"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="84"/>
+      <c r="Q14" s="54"/>
+      <c r="R14" s="55"/>
+      <c r="S14" s="56"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B15" s="88"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="22" t="s">
+      <c r="B15" s="39"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="10" t="s">
         <v>85</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -2373,1188 +2373,1177 @@
       <c r="I15" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="J15" s="36" t="s">
+      <c r="J15" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="K15" s="22" t="s">
+      <c r="K15" s="10" t="s">
         <v>98</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M15" s="23"/>
-      <c r="N15" s="83"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="90"/>
-      <c r="Q15" s="67"/>
-      <c r="R15" s="68"/>
-      <c r="S15" s="69"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="80"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="85"/>
+      <c r="Q15" s="54"/>
+      <c r="R15" s="55"/>
+      <c r="S15" s="56"/>
     </row>
     <row r="16" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="25"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="25" t="s">
+      <c r="B16" s="13"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G16" s="26" t="s">
+      <c r="G16" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26" t="s">
+      <c r="H16" s="14"/>
+      <c r="I16" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="J16" s="38" t="s">
+      <c r="J16" s="22" t="s">
         <v>94</v>
       </c>
-      <c r="K16" s="25" t="s">
+      <c r="K16" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="L16" s="26" t="s">
-        <v>203</v>
-      </c>
-      <c r="M16" s="27"/>
-      <c r="N16" s="84"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="70"/>
-      <c r="R16" s="71"/>
-      <c r="S16" s="72"/>
+      <c r="L16" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="M16" s="15"/>
+      <c r="N16" s="81"/>
+      <c r="O16" s="83"/>
+      <c r="P16" s="86"/>
+      <c r="Q16" s="57"/>
+      <c r="R16" s="58"/>
+      <c r="S16" s="59"/>
     </row>
     <row r="17" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="P17" s="29"/>
+      <c r="P17" s="16"/>
     </row>
     <row r="18" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="41" t="s">
-        <v>188</v>
-      </c>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="49"/>
-      <c r="L18" s="49"/>
-      <c r="M18" s="49"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="42"/>
-      <c r="P18" s="42"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="42"/>
-      <c r="S18" s="43"/>
+      <c r="C18" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="47"/>
+      <c r="O18" s="47"/>
+      <c r="P18" s="47"/>
+      <c r="Q18" s="47"/>
+      <c r="R18" s="47"/>
+      <c r="S18" s="49"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="19" t="s">
+      <c r="E19" s="73"/>
+      <c r="F19" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H19" s="20" t="s">
+      <c r="H19" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="N19" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="P19" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q19" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="I19" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="J19" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="L19" s="20" t="s">
-        <v>197</v>
-      </c>
-      <c r="M19" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="N19" s="81" t="s">
-        <v>3</v>
-      </c>
-      <c r="O19" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="P19" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q19" s="61" t="s">
-        <v>164</v>
-      </c>
-      <c r="R19" s="62"/>
-      <c r="S19" s="63"/>
+      <c r="R19" s="61"/>
+      <c r="S19" s="62"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="22" t="s">
+      <c r="E20" s="74"/>
+      <c r="F20" s="10" t="s">
         <v>74</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="J20" s="36" t="s">
+      <c r="J20" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="K20" s="22" t="s">
+      <c r="K20" s="10" t="s">
         <v>98</v>
       </c>
       <c r="L20" s="1"/>
-      <c r="M20" s="23" t="s">
+      <c r="M20" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="N20" s="18" t="s">
+      <c r="N20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O20" s="28" t="s">
+      <c r="O20" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="P20" s="74" t="s">
-        <v>189</v>
-      </c>
-      <c r="Q20" s="64"/>
-      <c r="R20" s="65"/>
-      <c r="S20" s="66"/>
+      <c r="P20" s="68" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q20" s="51"/>
+      <c r="R20" s="52"/>
+      <c r="S20" s="53"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="22" t="s">
+      <c r="E21" s="74"/>
+      <c r="F21" s="10" t="s">
         <v>76</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I21" s="16" t="s">
+      <c r="I21" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="J21" s="36" t="s">
+      <c r="J21" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="K21" s="22" t="s">
-        <v>184</v>
+      <c r="K21" s="10" t="s">
+        <v>183</v>
       </c>
       <c r="L21" s="1"/>
-      <c r="M21" s="23" t="s">
+      <c r="M21" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="N21" s="46" t="s">
+      <c r="N21" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="O21" s="28"/>
-      <c r="P21" s="74"/>
-      <c r="Q21" s="67"/>
-      <c r="R21" s="68"/>
-      <c r="S21" s="69"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="68"/>
+      <c r="Q21" s="54"/>
+      <c r="R21" s="55"/>
+      <c r="S21" s="56"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B22" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="23" t="s">
+      <c r="B22" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="44"/>
+      <c r="D22" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="22" t="s">
+      <c r="E22" s="74"/>
+      <c r="F22" s="10" t="s">
         <v>76</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I22" s="16" t="s">
+      <c r="I22" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="J22" s="36" t="s">
+      <c r="J22" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="K22" s="22" t="s">
-        <v>184</v>
+      <c r="K22" s="10" t="s">
+        <v>183</v>
       </c>
       <c r="L22" s="1"/>
-      <c r="M22" s="23" t="s">
+      <c r="M22" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="N22" s="46" t="s">
+      <c r="N22" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="O22" s="28"/>
-      <c r="P22" s="74"/>
-      <c r="Q22" s="67"/>
-      <c r="R22" s="68"/>
-      <c r="S22" s="69"/>
+      <c r="O22" s="44"/>
+      <c r="P22" s="68"/>
+      <c r="Q22" s="54"/>
+      <c r="R22" s="55"/>
+      <c r="S22" s="56"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="23" t="s">
+      <c r="C23" s="44"/>
+      <c r="D23" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="22" t="s">
+      <c r="E23" s="74"/>
+      <c r="F23" s="10" t="s">
         <v>74</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I23" s="16"/>
-      <c r="J23" s="36" t="s">
+      <c r="I23" s="5"/>
+      <c r="J23" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="K23" s="22" t="s">
-        <v>184</v>
+      <c r="K23" s="10" t="s">
+        <v>183</v>
       </c>
       <c r="L23" s="1"/>
-      <c r="M23" s="23" t="s">
+      <c r="M23" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="N23" s="46" t="s">
+      <c r="N23" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="O23" s="28"/>
-      <c r="P23" s="74"/>
-      <c r="Q23" s="67"/>
-      <c r="R23" s="68"/>
-      <c r="S23" s="69"/>
+      <c r="O23" s="44"/>
+      <c r="P23" s="68"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="55"/>
+      <c r="S23" s="56"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B24" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D24" s="23" t="s">
+      <c r="B24" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>176</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="22" t="s">
+      <c r="E24" s="74"/>
+      <c r="F24" s="10" t="s">
         <v>74</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I24" s="16"/>
-      <c r="J24" s="36" t="s">
+      <c r="I24" s="5"/>
+      <c r="J24" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="K24" s="22" t="s">
-        <v>184</v>
+      <c r="K24" s="10" t="s">
+        <v>183</v>
       </c>
       <c r="L24" s="1"/>
-      <c r="M24" s="23" t="s">
+      <c r="M24" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="N24" s="46" t="s">
+      <c r="N24" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="O24" s="28"/>
-      <c r="P24" s="74"/>
-      <c r="Q24" s="67"/>
-      <c r="R24" s="68"/>
-      <c r="S24" s="69"/>
+      <c r="O24" s="44"/>
+      <c r="P24" s="68"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="55"/>
+      <c r="S24" s="56"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B25" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="23" t="s">
+      <c r="B25" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="42"/>
+      <c r="D25" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="17"/>
-      <c r="F25" s="22" t="s">
+      <c r="E25" s="74"/>
+      <c r="F25" s="10" t="s">
         <v>74</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="I25" s="16" t="s">
-        <v>177</v>
-      </c>
-      <c r="J25" s="36" t="s">
+      <c r="I25" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="J25" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="K25" s="22" t="s">
+      <c r="K25" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O25" s="44"/>
+      <c r="P25" s="68"/>
+      <c r="Q25" s="54"/>
+      <c r="R25" s="55"/>
+      <c r="S25" s="56"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B26" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26" s="43"/>
+      <c r="D26" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="74"/>
+      <c r="F26" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="G26" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="L25" s="1"/>
-      <c r="M25" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="N25" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="O25" s="28"/>
-      <c r="P25" s="74"/>
-      <c r="Q25" s="67"/>
-      <c r="R25" s="68"/>
-      <c r="S25" s="69"/>
-    </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B26" s="22" t="s">
+      <c r="H26" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="K26" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="22" t="s">
+      <c r="L26" s="1"/>
+      <c r="M26" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O26" s="44"/>
+      <c r="P26" s="68"/>
+      <c r="Q26" s="54"/>
+      <c r="R26" s="55"/>
+      <c r="S26" s="56"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B27" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="E27" s="74"/>
+      <c r="F27" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G26" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="I26" s="1"/>
-      <c r="J26" s="36" t="s">
+      <c r="I27" s="1"/>
+      <c r="J27" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="K26" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="L26" s="1"/>
-      <c r="M26" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="N26" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="O26" s="28"/>
-      <c r="P26" s="74"/>
-      <c r="Q26" s="67"/>
-      <c r="R26" s="68"/>
-      <c r="S26" s="69"/>
-    </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B27" s="22" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="23" t="s">
+      <c r="K27" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="L27" s="1"/>
+      <c r="M27" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="N27" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="O27" s="44"/>
+      <c r="P27" s="68"/>
+      <c r="Q27" s="54"/>
+      <c r="R27" s="55"/>
+      <c r="S27" s="56"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.15">
+      <c r="B28" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="44"/>
+      <c r="D28" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E27" s="17"/>
-      <c r="F27" s="22" t="s">
+      <c r="E28" s="74"/>
+      <c r="F28" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G28" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="I27" s="1"/>
-      <c r="J27" s="36" t="s">
+      <c r="H28" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="I28" s="32"/>
+      <c r="J28" s="36" t="s">
         <v>130</v>
       </c>
-      <c r="K27" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="L27" s="1"/>
-      <c r="M27" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="N27" s="46" t="s">
-        <v>34</v>
-      </c>
-      <c r="O27" s="28"/>
-      <c r="P27" s="74"/>
-      <c r="Q27" s="67"/>
-      <c r="R27" s="68"/>
-      <c r="S27" s="69"/>
-    </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B28" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" s="28"/>
-      <c r="D28" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="77" t="s">
-        <v>74</v>
-      </c>
-      <c r="G28" s="78" t="s">
-        <v>187</v>
-      </c>
-      <c r="H28" s="78" t="s">
-        <v>175</v>
-      </c>
-      <c r="I28" s="78"/>
-      <c r="J28" s="85" t="s">
-        <v>130</v>
-      </c>
-      <c r="K28" s="77" t="s">
-        <v>184</v>
-      </c>
-      <c r="L28" s="78"/>
-      <c r="M28" s="79" t="s">
+      <c r="K28" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="L28" s="32"/>
+      <c r="M28" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="N28" s="86" t="s">
+      <c r="N28" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="O28" s="28"/>
-      <c r="P28" s="74"/>
-      <c r="Q28" s="67"/>
-      <c r="R28" s="68"/>
-      <c r="S28" s="69"/>
+      <c r="O28" s="44"/>
+      <c r="P28" s="68"/>
+      <c r="Q28" s="54"/>
+      <c r="R28" s="55"/>
+      <c r="S28" s="56"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B29" s="22"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="22" t="s">
+      <c r="B29" s="10"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="10" t="s">
         <v>85</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>133</v>
       </c>
       <c r="I29" s="1"/>
-      <c r="J29" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="K29" s="22" t="s">
+      <c r="J29" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="K29" s="10" t="s">
         <v>98</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="M29" s="23"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="M29" s="11"/>
+      <c r="N29" s="25"/>
+      <c r="O29" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="P29" s="74"/>
-      <c r="Q29" s="67"/>
-      <c r="R29" s="68"/>
-      <c r="S29" s="69"/>
+      <c r="P29" s="68"/>
+      <c r="Q29" s="54"/>
+      <c r="R29" s="55"/>
+      <c r="S29" s="56"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" s="23" t="s">
+      <c r="C30" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="D30" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="22" t="s">
+      <c r="E30" s="74"/>
+      <c r="F30" s="10" t="s">
         <v>85</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>133</v>
       </c>
       <c r="I30" s="1"/>
-      <c r="J30" s="36" t="s">
+      <c r="J30" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="K30" s="22" t="s">
+      <c r="K30" s="10" t="s">
         <v>98</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M30" s="23"/>
-      <c r="N30" s="46"/>
-      <c r="O30" s="8"/>
-      <c r="P30" s="74"/>
-      <c r="Q30" s="67"/>
-      <c r="R30" s="68"/>
-      <c r="S30" s="69"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="68"/>
+      <c r="Q30" s="54"/>
+      <c r="R30" s="55"/>
+      <c r="S30" s="56"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="23" t="s">
+      <c r="C31" s="42"/>
+      <c r="D31" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="22" t="s">
+      <c r="E31" s="74"/>
+      <c r="F31" s="10" t="s">
         <v>85</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>133</v>
       </c>
       <c r="I31" s="1"/>
-      <c r="J31" s="36" t="s">
+      <c r="J31" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="K31" s="22" t="s">
+      <c r="K31" s="10" t="s">
         <v>98</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M31" s="23"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="8"/>
-      <c r="P31" s="74"/>
-      <c r="Q31" s="67"/>
-      <c r="R31" s="68"/>
-      <c r="S31" s="69"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="25"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="68"/>
+      <c r="Q31" s="54"/>
+      <c r="R31" s="55"/>
+      <c r="S31" s="56"/>
     </row>
     <row r="32" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="C32" s="45"/>
+      <c r="D32" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="27" t="s">
-        <v>180</v>
-      </c>
-      <c r="E32" s="51"/>
-      <c r="F32" s="25" t="s">
+      <c r="E32" s="75"/>
+      <c r="F32" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G32" s="26" t="s">
+      <c r="G32" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="J32" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="J32" s="38" t="s">
-        <v>170</v>
-      </c>
-      <c r="K32" s="25" t="s">
+      <c r="K32" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="L32" s="26" t="s">
+      <c r="L32" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="M32" s="27"/>
-      <c r="N32" s="87"/>
-      <c r="O32" s="52"/>
-      <c r="P32" s="75"/>
-      <c r="Q32" s="70"/>
-      <c r="R32" s="71"/>
-      <c r="S32" s="72"/>
+      <c r="M32" s="15"/>
+      <c r="N32" s="38"/>
+      <c r="O32" s="45"/>
+      <c r="P32" s="69"/>
+      <c r="Q32" s="57"/>
+      <c r="R32" s="58"/>
+      <c r="S32" s="59"/>
     </row>
     <row r="33" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="42"/>
-      <c r="E34" s="42"/>
-      <c r="F34" s="42"/>
-      <c r="G34" s="42"/>
-      <c r="H34" s="42"/>
-      <c r="I34" s="42"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="42"/>
-      <c r="L34" s="42"/>
-      <c r="M34" s="42"/>
-      <c r="N34" s="42"/>
-      <c r="O34" s="42"/>
-      <c r="P34" s="42"/>
-      <c r="Q34" s="42"/>
-      <c r="R34" s="42"/>
-      <c r="S34" s="43"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="47"/>
+      <c r="P34" s="47"/>
+      <c r="Q34" s="47"/>
+      <c r="R34" s="47"/>
+      <c r="S34" s="49"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="54"/>
-      <c r="F35" s="19" t="s">
+      <c r="E35" s="65"/>
+      <c r="F35" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="G35" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="H35" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="L35" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="M35" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O35" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="P35" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q35" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="I35" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="J35" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="K35" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="L35" s="47" t="s">
-        <v>197</v>
-      </c>
-      <c r="M35" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="N35" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="O35" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="P35" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q35" s="61" t="s">
-        <v>164</v>
-      </c>
-      <c r="R35" s="62"/>
-      <c r="S35" s="63"/>
+      <c r="R35" s="61"/>
+      <c r="S35" s="62"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D36" s="23" t="s">
+      <c r="D36" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="55"/>
-      <c r="F36" s="22"/>
+      <c r="E36" s="66"/>
+      <c r="F36" s="10"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="23"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="23" t="s">
+      <c r="J36" s="11"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="N36" s="22" t="s">
+      <c r="N36" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="O36" s="28" t="s">
+      <c r="O36" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="P36" s="32" t="s">
+      <c r="P36" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="Q36" s="64"/>
-      <c r="R36" s="65"/>
-      <c r="S36" s="66"/>
+      <c r="Q36" s="51"/>
+      <c r="R36" s="52"/>
+      <c r="S36" s="53"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="D37" s="23" t="s">
+      <c r="D37" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="55"/>
-      <c r="F37" s="22"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="10"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-      <c r="I37" s="16"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="23" t="s">
+      <c r="I37" s="5"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="N37" s="40" t="s">
+      <c r="N37" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="O37" s="28"/>
-      <c r="P37" s="32"/>
-      <c r="Q37" s="67"/>
-      <c r="R37" s="68"/>
-      <c r="S37" s="69"/>
+      <c r="O37" s="44"/>
+      <c r="P37" s="71"/>
+      <c r="Q37" s="54"/>
+      <c r="R37" s="55"/>
+      <c r="S37" s="56"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B38" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="23" t="s">
+      <c r="B38" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="C38" s="42"/>
+      <c r="D38" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E38" s="55"/>
-      <c r="F38" s="22"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="10"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-      <c r="I38" s="16"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="34"/>
-      <c r="M38" s="23" t="s">
+      <c r="I38" s="5"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="N38" s="22" t="s">
+      <c r="N38" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="O38" s="28"/>
-      <c r="P38" s="32"/>
-      <c r="Q38" s="67"/>
-      <c r="R38" s="68"/>
-      <c r="S38" s="69"/>
+      <c r="O38" s="44"/>
+      <c r="P38" s="71"/>
+      <c r="Q38" s="54"/>
+      <c r="R38" s="55"/>
+      <c r="S38" s="56"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B39" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="23" t="s">
+      <c r="B39" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" s="42"/>
+      <c r="D39" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="55"/>
-      <c r="F39" s="22"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="10"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-      <c r="I39" s="16"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="23" t="s">
+      <c r="I39" s="5"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="N39" s="22" t="s">
+      <c r="N39" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="O39" s="28"/>
-      <c r="P39" s="32"/>
-      <c r="Q39" s="67"/>
-      <c r="R39" s="68"/>
-      <c r="S39" s="69"/>
+      <c r="O39" s="44"/>
+      <c r="P39" s="71"/>
+      <c r="Q39" s="54"/>
+      <c r="R39" s="55"/>
+      <c r="S39" s="56"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B40" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="23" t="s">
+      <c r="B40" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" s="42"/>
+      <c r="D40" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E40" s="55"/>
-      <c r="F40" s="22"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="10"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="34"/>
-      <c r="M40" s="23" t="s">
+      <c r="I40" s="5"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="N40" s="22" t="s">
+      <c r="N40" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="O40" s="28"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="67"/>
-      <c r="R40" s="68"/>
-      <c r="S40" s="69"/>
+      <c r="O40" s="44"/>
+      <c r="P40" s="71"/>
+      <c r="Q40" s="54"/>
+      <c r="R40" s="55"/>
+      <c r="S40" s="56"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B41" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="23" t="s">
+      <c r="B41" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" s="42"/>
+      <c r="D41" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E41" s="55"/>
-      <c r="F41" s="22"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="10"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-      <c r="I41" s="16"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="34"/>
-      <c r="M41" s="23" t="s">
+      <c r="I41" s="5"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="N41" s="22" t="s">
+      <c r="N41" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="O41" s="28"/>
-      <c r="P41" s="32"/>
-      <c r="Q41" s="67"/>
-      <c r="R41" s="68"/>
-      <c r="S41" s="69"/>
+      <c r="O41" s="44"/>
+      <c r="P41" s="71"/>
+      <c r="Q41" s="54"/>
+      <c r="R41" s="55"/>
+      <c r="S41" s="56"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B42" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="23" t="s">
+      <c r="B42" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C42" s="43"/>
+      <c r="D42" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E42" s="55"/>
-      <c r="F42" s="22"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="10"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="23"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="34"/>
-      <c r="M42" s="23" t="s">
+      <c r="J42" s="11"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="N42" s="22" t="s">
+      <c r="N42" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="O42" s="28"/>
-      <c r="P42" s="32"/>
-      <c r="Q42" s="67"/>
-      <c r="R42" s="68"/>
-      <c r="S42" s="69"/>
+      <c r="O42" s="44"/>
+      <c r="P42" s="71"/>
+      <c r="Q42" s="54"/>
+      <c r="R42" s="55"/>
+      <c r="S42" s="56"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B43" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="C43" s="10" t="s">
+      <c r="B43" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D43" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E43" s="55"/>
-      <c r="F43" s="22"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="10"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="34"/>
-      <c r="M43" s="23" t="s">
+      <c r="J43" s="11"/>
+      <c r="K43" s="10"/>
+      <c r="L43" s="18"/>
+      <c r="M43" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="N43" s="40" t="s">
+      <c r="N43" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="O43" s="28"/>
-      <c r="P43" s="32"/>
-      <c r="Q43" s="67"/>
-      <c r="R43" s="68"/>
-      <c r="S43" s="69"/>
+      <c r="O43" s="44"/>
+      <c r="P43" s="71"/>
+      <c r="Q43" s="54"/>
+      <c r="R43" s="55"/>
+      <c r="S43" s="56"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B44" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="C44" s="10" t="s">
+      <c r="B44" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D44" s="23" t="s">
+      <c r="D44" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E44" s="55"/>
-      <c r="F44" s="22"/>
+      <c r="E44" s="66"/>
+      <c r="F44" s="10"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="34"/>
-      <c r="M44" s="23" t="s">
+      <c r="J44" s="11"/>
+      <c r="K44" s="10"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="N44" s="40" t="s">
+      <c r="N44" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="O44" s="28"/>
-      <c r="P44" s="32"/>
-      <c r="Q44" s="67"/>
-      <c r="R44" s="68"/>
-      <c r="S44" s="69"/>
+      <c r="O44" s="44"/>
+      <c r="P44" s="71"/>
+      <c r="Q44" s="54"/>
+      <c r="R44" s="55"/>
+      <c r="S44" s="56"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C45" s="28" t="s">
+      <c r="C45" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E45" s="55"/>
-      <c r="F45" s="22"/>
+      <c r="E45" s="66"/>
+      <c r="F45" s="10"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="34"/>
-      <c r="M45" s="23" t="s">
+      <c r="J45" s="11"/>
+      <c r="K45" s="10"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="N45" s="40" t="s">
+      <c r="N45" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="O45" s="28"/>
-      <c r="P45" s="32"/>
-      <c r="Q45" s="67"/>
-      <c r="R45" s="68"/>
-      <c r="S45" s="69"/>
+      <c r="O45" s="44"/>
+      <c r="P45" s="71"/>
+      <c r="Q45" s="54"/>
+      <c r="R45" s="55"/>
+      <c r="S45" s="56"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="23" t="s">
+      <c r="C46" s="44"/>
+      <c r="D46" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E46" s="55"/>
-      <c r="F46" s="22"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="10"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="23"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="34"/>
-      <c r="M46" s="23" t="s">
+      <c r="J46" s="11"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="N46" s="40" t="s">
+      <c r="N46" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="O46" s="28"/>
-      <c r="P46" s="32"/>
-      <c r="Q46" s="67"/>
-      <c r="R46" s="68"/>
-      <c r="S46" s="69"/>
+      <c r="O46" s="44"/>
+      <c r="P46" s="71"/>
+      <c r="Q46" s="54"/>
+      <c r="R46" s="55"/>
+      <c r="S46" s="56"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="C47" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D47" s="23" t="s">
+      <c r="C47" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="E47" s="55"/>
-      <c r="F47" s="22"/>
+      <c r="E47" s="66"/>
+      <c r="F47" s="10"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="22"/>
-      <c r="L47" s="34"/>
-      <c r="M47" s="23" t="s">
+      <c r="J47" s="11"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="N47" s="40" t="s">
+      <c r="N47" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="O47" s="28"/>
-      <c r="P47" s="32"/>
-      <c r="Q47" s="67"/>
-      <c r="R47" s="68"/>
-      <c r="S47" s="69"/>
+      <c r="O47" s="44"/>
+      <c r="P47" s="71"/>
+      <c r="Q47" s="54"/>
+      <c r="R47" s="55"/>
+      <c r="S47" s="56"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="23" t="s">
+      <c r="C48" s="42"/>
+      <c r="D48" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="E48" s="55"/>
-      <c r="F48" s="22"/>
+      <c r="E48" s="66"/>
+      <c r="F48" s="10"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="23"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="34"/>
-      <c r="M48" s="23" t="s">
+      <c r="J48" s="11"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="N48" s="22" t="s">
+      <c r="N48" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="O48" s="28"/>
-      <c r="P48" s="32"/>
-      <c r="Q48" s="67"/>
-      <c r="R48" s="68"/>
-      <c r="S48" s="69"/>
+      <c r="O48" s="44"/>
+      <c r="P48" s="71"/>
+      <c r="Q48" s="54"/>
+      <c r="R48" s="55"/>
+      <c r="S48" s="56"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="23"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="22"/>
+      <c r="C49" s="42"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="10"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="34"/>
-      <c r="M49" s="23" t="s">
+      <c r="J49" s="11"/>
+      <c r="K49" s="10"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="N49" s="22" t="s">
+      <c r="N49" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="O49" s="28"/>
-      <c r="P49" s="32"/>
-      <c r="Q49" s="67"/>
-      <c r="R49" s="68"/>
-      <c r="S49" s="69"/>
+      <c r="O49" s="44"/>
+      <c r="P49" s="71"/>
+      <c r="Q49" s="54"/>
+      <c r="R49" s="55"/>
+      <c r="S49" s="56"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="23"/>
-      <c r="E50" s="55"/>
-      <c r="F50" s="22"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="10"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="23"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="34" t="s">
+      <c r="J50" s="11"/>
+      <c r="K50" s="10"/>
+      <c r="L50" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="M50" s="23"/>
-      <c r="N50" s="57" t="s">
+      <c r="M50" s="11"/>
+      <c r="N50" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="O50" s="28" t="s">
+      <c r="O50" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="P50" s="32"/>
-      <c r="Q50" s="67"/>
-      <c r="R50" s="68"/>
-      <c r="S50" s="69"/>
+      <c r="P50" s="71"/>
+      <c r="Q50" s="54"/>
+      <c r="R50" s="55"/>
+      <c r="S50" s="56"/>
     </row>
     <row r="51" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="25"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="26"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="25"/>
-      <c r="L51" s="35" t="s">
+      <c r="B51" s="13"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="15"/>
+      <c r="E51" s="67"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="15"/>
+      <c r="K51" s="13"/>
+      <c r="L51" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="M51" s="27"/>
-      <c r="N51" s="58"/>
-      <c r="O51" s="59"/>
-      <c r="P51" s="33"/>
-      <c r="Q51" s="70"/>
-      <c r="R51" s="71"/>
-      <c r="S51" s="72"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="64"/>
+      <c r="O51" s="70"/>
+      <c r="P51" s="72"/>
+      <c r="Q51" s="57"/>
+      <c r="R51" s="58"/>
+      <c r="S51" s="59"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="N52" s="53"/>
+      <c r="N52" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="O29:O32"/>
-    <mergeCell ref="C18:S18"/>
-    <mergeCell ref="C2:S2"/>
-    <mergeCell ref="C34:S34"/>
-    <mergeCell ref="Q4:S16"/>
-    <mergeCell ref="Q20:S32"/>
     <mergeCell ref="Q36:S51"/>
     <mergeCell ref="Q35:S35"/>
     <mergeCell ref="Q19:S19"/>
     <mergeCell ref="C47:C50"/>
     <mergeCell ref="N50:N51"/>
-    <mergeCell ref="Q3:S3"/>
     <mergeCell ref="E35:E51"/>
     <mergeCell ref="P20:P32"/>
     <mergeCell ref="O20:O28"/>
@@ -3564,6 +3553,12 @@
     <mergeCell ref="E19:E32"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C18:S18"/>
+    <mergeCell ref="C2:S2"/>
+    <mergeCell ref="C34:S34"/>
+    <mergeCell ref="Q4:S16"/>
+    <mergeCell ref="Q20:S32"/>
+    <mergeCell ref="Q3:S3"/>
     <mergeCell ref="C5:C10"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="C13:C14"/>
@@ -3572,6 +3567,11 @@
     <mergeCell ref="E3:E16"/>
     <mergeCell ref="O4:O11"/>
     <mergeCell ref="P4:P16"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="O29:O32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3598,22 +3598,22 @@
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
+      <c r="G2" s="88"/>
+      <c r="H2" s="89"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3629,33 +3629,33 @@
         <v>68</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="10"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
         <v>70</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="10"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B10" s="1"/>
@@ -3665,27 +3665,27 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="10"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="10"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="10"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B16" s="1"/>
@@ -3733,22 +3733,22 @@
       <c r="A2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3760,27 +3760,27 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="10"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="10"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="10"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="10"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B10" s="1"/>
@@ -3790,27 +3790,27 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="10"/>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="10"/>
+      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="10"/>
+      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="10"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="10"/>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B16" s="1"/>

</xml_diff>

<commit_message>
Added the Tracke and the Ride modules to the project
</commit_message>
<xml_diff>
--- a/doc/BikeRide-Model.xlsx
+++ b/doc/BikeRide-Model.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="204">
   <si>
     <t>Biker</t>
   </si>
@@ -1291,66 +1291,108 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1379,48 +1421,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1822,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -1852,25 +1852,25 @@
       <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="49"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="47"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B3" s="7" t="s">
@@ -1882,7 +1882,7 @@
       <c r="D3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="73"/>
+      <c r="E3" s="70"/>
       <c r="F3" s="7" t="s">
         <v>72</v>
       </c>
@@ -1916,11 +1916,11 @@
       <c r="P3" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="Q3" s="60" t="s">
+      <c r="Q3" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="R3" s="61"/>
-      <c r="S3" s="62"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="60"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B4" s="10" t="s">
@@ -1932,7 +1932,7 @@
       <c r="D4" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="74"/>
+      <c r="E4" s="71"/>
       <c r="F4" s="10" t="s">
         <v>74</v>
       </c>
@@ -1956,27 +1956,27 @@
       <c r="N4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="44" t="s">
+      <c r="O4" s="61" t="s">
         <v>135</v>
       </c>
-      <c r="P4" s="84" t="s">
+      <c r="P4" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="52"/>
-      <c r="S4" s="53"/>
+      <c r="Q4" s="49"/>
+      <c r="R4" s="50"/>
+      <c r="S4" s="51"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B5" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="44" t="s">
+      <c r="C5" s="61" t="s">
         <v>90</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="74"/>
+      <c r="E5" s="71"/>
       <c r="F5" s="10" t="s">
         <v>76</v>
       </c>
@@ -2002,21 +2002,21 @@
       <c r="N5" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="O5" s="44"/>
-      <c r="P5" s="84"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="55"/>
-      <c r="S5" s="56"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="73"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="53"/>
+      <c r="S5" s="54"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B6" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="44"/>
+      <c r="C6" s="61"/>
       <c r="D6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="74"/>
+      <c r="E6" s="71"/>
       <c r="F6" s="10" t="s">
         <v>76</v>
       </c>
@@ -2042,21 +2042,21 @@
       <c r="N6" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="O6" s="44"/>
-      <c r="P6" s="84"/>
-      <c r="Q6" s="54"/>
-      <c r="R6" s="55"/>
-      <c r="S6" s="56"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="73"/>
+      <c r="Q6" s="52"/>
+      <c r="R6" s="53"/>
+      <c r="S6" s="54"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B7" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="44"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="74"/>
+      <c r="E7" s="71"/>
       <c r="F7" s="10" t="s">
         <v>76</v>
       </c>
@@ -2082,21 +2082,21 @@
       <c r="N7" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="44"/>
-      <c r="P7" s="84"/>
-      <c r="Q7" s="54"/>
-      <c r="R7" s="55"/>
-      <c r="S7" s="56"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="53"/>
+      <c r="S7" s="54"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B8" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="44"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="74"/>
+      <c r="E8" s="71"/>
       <c r="F8" s="10" t="s">
         <v>76</v>
       </c>
@@ -2122,21 +2122,21 @@
       <c r="N8" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="O8" s="44"/>
-      <c r="P8" s="84"/>
-      <c r="Q8" s="54"/>
-      <c r="R8" s="55"/>
-      <c r="S8" s="56"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="52"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="54"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B9" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="44"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="74"/>
+      <c r="E9" s="71"/>
       <c r="F9" s="10" t="s">
         <v>76</v>
       </c>
@@ -2162,21 +2162,21 @@
       <c r="N9" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="O9" s="44"/>
-      <c r="P9" s="84"/>
-      <c r="Q9" s="54"/>
-      <c r="R9" s="55"/>
-      <c r="S9" s="56"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="73"/>
+      <c r="Q9" s="52"/>
+      <c r="R9" s="53"/>
+      <c r="S9" s="54"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B10" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="44"/>
+      <c r="C10" s="61"/>
       <c r="D10" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="74"/>
+      <c r="E10" s="71"/>
       <c r="F10" s="10" t="s">
         <v>74</v>
       </c>
@@ -2200,23 +2200,17 @@
       <c r="N10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O10" s="44"/>
-      <c r="P10" s="84"/>
-      <c r="Q10" s="54"/>
-      <c r="R10" s="55"/>
-      <c r="S10" s="56"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="73"/>
+      <c r="Q10" s="52"/>
+      <c r="R10" s="53"/>
+      <c r="S10" s="54"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B11" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11" s="76" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E11" s="74"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="71"/>
       <c r="F11" s="10" t="s">
         <v>74</v>
       </c>
@@ -2240,21 +2234,17 @@
       <c r="N11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="O11" s="44"/>
-      <c r="P11" s="84"/>
-      <c r="Q11" s="54"/>
-      <c r="R11" s="55"/>
-      <c r="S11" s="56"/>
+      <c r="O11" s="61"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="52"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="54"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B12" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C12" s="76"/>
-      <c r="D12" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E12" s="74"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="71"/>
       <c r="F12" s="10" t="s">
         <v>85</v>
       </c>
@@ -2275,26 +2265,26 @@
         <v>194</v>
       </c>
       <c r="M12" s="11"/>
-      <c r="N12" s="79"/>
-      <c r="O12" s="77" t="s">
+      <c r="N12" s="65"/>
+      <c r="O12" s="63" t="s">
         <v>136</v>
       </c>
-      <c r="P12" s="84"/>
-      <c r="Q12" s="54"/>
-      <c r="R12" s="55"/>
-      <c r="S12" s="56"/>
+      <c r="P12" s="73"/>
+      <c r="Q12" s="52"/>
+      <c r="R12" s="53"/>
+      <c r="S12" s="54"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B13" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="63" t="s">
         <v>156</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="74"/>
+      <c r="E13" s="71"/>
       <c r="F13" s="10" t="s">
         <v>85</v>
       </c>
@@ -2315,22 +2305,22 @@
         <v>198</v>
       </c>
       <c r="M13" s="11"/>
-      <c r="N13" s="80"/>
-      <c r="O13" s="82"/>
-      <c r="P13" s="84"/>
-      <c r="Q13" s="54"/>
-      <c r="R13" s="55"/>
-      <c r="S13" s="56"/>
+      <c r="N13" s="66"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="73"/>
+      <c r="Q13" s="52"/>
+      <c r="R13" s="53"/>
+      <c r="S13" s="54"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B14" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="78"/>
+      <c r="C14" s="64"/>
       <c r="D14" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="74"/>
+      <c r="E14" s="71"/>
       <c r="F14" s="10" t="s">
         <v>85</v>
       </c>
@@ -2351,18 +2341,18 @@
         <v>12</v>
       </c>
       <c r="M14" s="11"/>
-      <c r="N14" s="80"/>
-      <c r="O14" s="82"/>
-      <c r="P14" s="84"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="55"/>
-      <c r="S14" s="56"/>
+      <c r="N14" s="66"/>
+      <c r="O14" s="68"/>
+      <c r="P14" s="73"/>
+      <c r="Q14" s="52"/>
+      <c r="R14" s="53"/>
+      <c r="S14" s="54"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B15" s="39"/>
       <c r="C15" s="29"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="74"/>
+      <c r="E15" s="71"/>
       <c r="F15" s="10" t="s">
         <v>85</v>
       </c>
@@ -2383,18 +2373,18 @@
         <v>13</v>
       </c>
       <c r="M15" s="11"/>
-      <c r="N15" s="80"/>
-      <c r="O15" s="82"/>
-      <c r="P15" s="85"/>
-      <c r="Q15" s="54"/>
-      <c r="R15" s="55"/>
-      <c r="S15" s="56"/>
+      <c r="N15" s="66"/>
+      <c r="O15" s="68"/>
+      <c r="P15" s="74"/>
+      <c r="Q15" s="52"/>
+      <c r="R15" s="53"/>
+      <c r="S15" s="54"/>
     </row>
     <row r="16" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="13"/>
       <c r="C16" s="24"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="75"/>
+      <c r="E16" s="72"/>
       <c r="F16" s="13" t="s">
         <v>85</v>
       </c>
@@ -2415,12 +2405,12 @@
         <v>202</v>
       </c>
       <c r="M16" s="15"/>
-      <c r="N16" s="81"/>
-      <c r="O16" s="83"/>
-      <c r="P16" s="86"/>
-      <c r="Q16" s="57"/>
-      <c r="R16" s="58"/>
-      <c r="S16" s="59"/>
+      <c r="N16" s="67"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="75"/>
+      <c r="Q16" s="55"/>
+      <c r="R16" s="56"/>
+      <c r="S16" s="57"/>
     </row>
     <row r="17" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="P17" s="16"/>
@@ -2429,25 +2419,25 @@
       <c r="B18" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="47"/>
-      <c r="P18" s="47"/>
-      <c r="Q18" s="47"/>
-      <c r="R18" s="47"/>
-      <c r="S18" s="49"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="45"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="45"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="47"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B19" s="7" t="s">
@@ -2459,7 +2449,7 @@
       <c r="D19" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="73"/>
+      <c r="E19" s="70"/>
       <c r="F19" s="7" t="s">
         <v>72</v>
       </c>
@@ -2493,11 +2483,11 @@
       <c r="P19" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="Q19" s="60" t="s">
+      <c r="Q19" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="R19" s="61"/>
-      <c r="S19" s="62"/>
+      <c r="R19" s="59"/>
+      <c r="S19" s="60"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B20" s="10" t="s">
@@ -2509,7 +2499,7 @@
       <c r="D20" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="74"/>
+      <c r="E20" s="71"/>
       <c r="F20" s="10" t="s">
         <v>74</v>
       </c>
@@ -2533,27 +2523,27 @@
       <c r="N20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O20" s="44" t="s">
+      <c r="O20" s="61" t="s">
         <v>135</v>
       </c>
-      <c r="P20" s="68" t="s">
+      <c r="P20" s="82" t="s">
         <v>188</v>
       </c>
-      <c r="Q20" s="51"/>
-      <c r="R20" s="52"/>
-      <c r="S20" s="53"/>
+      <c r="Q20" s="49"/>
+      <c r="R20" s="50"/>
+      <c r="S20" s="51"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B21" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="44" t="s">
+      <c r="C21" s="61" t="s">
         <v>131</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="74"/>
+      <c r="E21" s="71"/>
       <c r="F21" s="10" t="s">
         <v>76</v>
       </c>
@@ -2579,21 +2569,21 @@
       <c r="N21" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="O21" s="44"/>
-      <c r="P21" s="68"/>
-      <c r="Q21" s="54"/>
-      <c r="R21" s="55"/>
-      <c r="S21" s="56"/>
+      <c r="O21" s="61"/>
+      <c r="P21" s="82"/>
+      <c r="Q21" s="52"/>
+      <c r="R21" s="53"/>
+      <c r="S21" s="54"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B22" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="C22" s="44"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E22" s="74"/>
+      <c r="E22" s="71"/>
       <c r="F22" s="10" t="s">
         <v>76</v>
       </c>
@@ -2619,21 +2609,21 @@
       <c r="N22" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="O22" s="44"/>
-      <c r="P22" s="68"/>
-      <c r="Q22" s="54"/>
-      <c r="R22" s="55"/>
-      <c r="S22" s="56"/>
+      <c r="O22" s="61"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="52"/>
+      <c r="R22" s="53"/>
+      <c r="S22" s="54"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B23" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="44"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="74"/>
+      <c r="E23" s="71"/>
       <c r="F23" s="10" t="s">
         <v>74</v>
       </c>
@@ -2657,11 +2647,11 @@
       <c r="N23" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="O23" s="44"/>
-      <c r="P23" s="68"/>
-      <c r="Q23" s="54"/>
-      <c r="R23" s="55"/>
-      <c r="S23" s="56"/>
+      <c r="O23" s="61"/>
+      <c r="P23" s="82"/>
+      <c r="Q23" s="52"/>
+      <c r="R23" s="53"/>
+      <c r="S23" s="54"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B24" s="10" t="s">
@@ -2673,7 +2663,7 @@
       <c r="D24" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="74"/>
+      <c r="E24" s="71"/>
       <c r="F24" s="10" t="s">
         <v>74</v>
       </c>
@@ -2697,11 +2687,11 @@
       <c r="N24" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="O24" s="44"/>
-      <c r="P24" s="68"/>
-      <c r="Q24" s="54"/>
-      <c r="R24" s="55"/>
-      <c r="S24" s="56"/>
+      <c r="O24" s="61"/>
+      <c r="P24" s="82"/>
+      <c r="Q24" s="52"/>
+      <c r="R24" s="53"/>
+      <c r="S24" s="54"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B25" s="10" t="s">
@@ -2711,7 +2701,7 @@
       <c r="D25" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="74"/>
+      <c r="E25" s="71"/>
       <c r="F25" s="10" t="s">
         <v>74</v>
       </c>
@@ -2737,21 +2727,21 @@
       <c r="N25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O25" s="44"/>
-      <c r="P25" s="68"/>
-      <c r="Q25" s="54"/>
-      <c r="R25" s="55"/>
-      <c r="S25" s="56"/>
+      <c r="O25" s="61"/>
+      <c r="P25" s="82"/>
+      <c r="Q25" s="52"/>
+      <c r="R25" s="53"/>
+      <c r="S25" s="54"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B26" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="C26" s="43"/>
+      <c r="C26" s="76"/>
       <c r="D26" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="74"/>
+      <c r="E26" s="71"/>
       <c r="F26" s="10" t="s">
         <v>173</v>
       </c>
@@ -2775,23 +2765,17 @@
       <c r="N26" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="O26" s="44"/>
-      <c r="P26" s="68"/>
-      <c r="Q26" s="54"/>
-      <c r="R26" s="55"/>
-      <c r="S26" s="56"/>
+      <c r="O26" s="61"/>
+      <c r="P26" s="82"/>
+      <c r="Q26" s="52"/>
+      <c r="R26" s="53"/>
+      <c r="S26" s="54"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B27" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E27" s="74"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="71"/>
       <c r="F27" s="10" t="s">
         <v>74</v>
       </c>
@@ -2815,21 +2799,17 @@
       <c r="N27" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="O27" s="44"/>
-      <c r="P27" s="68"/>
-      <c r="Q27" s="54"/>
-      <c r="R27" s="55"/>
-      <c r="S27" s="56"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="82"/>
+      <c r="Q27" s="52"/>
+      <c r="R27" s="53"/>
+      <c r="S27" s="54"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.15">
-      <c r="B28" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" s="44"/>
-      <c r="D28" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="E28" s="74"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="71"/>
       <c r="F28" s="31" t="s">
         <v>74</v>
       </c>
@@ -2853,17 +2833,17 @@
       <c r="N28" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="O28" s="44"/>
-      <c r="P28" s="68"/>
-      <c r="Q28" s="54"/>
-      <c r="R28" s="55"/>
-      <c r="S28" s="56"/>
+      <c r="O28" s="61"/>
+      <c r="P28" s="82"/>
+      <c r="Q28" s="52"/>
+      <c r="R28" s="53"/>
+      <c r="S28" s="54"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B29" s="10"/>
       <c r="C29" s="30"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="74"/>
+      <c r="E29" s="71"/>
       <c r="F29" s="10" t="s">
         <v>85</v>
       </c>
@@ -2888,10 +2868,10 @@
       <c r="O29" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="P29" s="68"/>
-      <c r="Q29" s="54"/>
-      <c r="R29" s="55"/>
-      <c r="S29" s="56"/>
+      <c r="P29" s="82"/>
+      <c r="Q29" s="52"/>
+      <c r="R29" s="53"/>
+      <c r="S29" s="54"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B30" s="10" t="s">
@@ -2903,7 +2883,7 @@
       <c r="D30" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E30" s="74"/>
+      <c r="E30" s="71"/>
       <c r="F30" s="10" t="s">
         <v>85</v>
       </c>
@@ -2926,10 +2906,10 @@
       <c r="M30" s="11"/>
       <c r="N30" s="25"/>
       <c r="O30" s="42"/>
-      <c r="P30" s="68"/>
-      <c r="Q30" s="54"/>
-      <c r="R30" s="55"/>
-      <c r="S30" s="56"/>
+      <c r="P30" s="82"/>
+      <c r="Q30" s="52"/>
+      <c r="R30" s="53"/>
+      <c r="S30" s="54"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B31" s="10" t="s">
@@ -2939,7 +2919,7 @@
       <c r="D31" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="74"/>
+      <c r="E31" s="71"/>
       <c r="F31" s="10" t="s">
         <v>85</v>
       </c>
@@ -2962,20 +2942,20 @@
       <c r="M31" s="11"/>
       <c r="N31" s="25"/>
       <c r="O31" s="42"/>
-      <c r="P31" s="68"/>
-      <c r="Q31" s="54"/>
-      <c r="R31" s="55"/>
-      <c r="S31" s="56"/>
+      <c r="P31" s="82"/>
+      <c r="Q31" s="52"/>
+      <c r="R31" s="53"/>
+      <c r="S31" s="54"/>
     </row>
     <row r="32" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B32" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="C32" s="45"/>
+      <c r="C32" s="43"/>
       <c r="D32" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="E32" s="75"/>
+      <c r="E32" s="72"/>
       <c r="F32" s="13" t="s">
         <v>85</v>
       </c>
@@ -2997,36 +2977,36 @@
       </c>
       <c r="M32" s="15"/>
       <c r="N32" s="38"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="69"/>
-      <c r="Q32" s="57"/>
-      <c r="R32" s="58"/>
-      <c r="S32" s="59"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="83"/>
+      <c r="Q32" s="55"/>
+      <c r="R32" s="56"/>
+      <c r="S32" s="57"/>
     </row>
     <row r="33" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B34" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="46" t="s">
+      <c r="C34" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="47"/>
-      <c r="O34" s="47"/>
-      <c r="P34" s="47"/>
-      <c r="Q34" s="47"/>
-      <c r="R34" s="47"/>
-      <c r="S34" s="49"/>
+      <c r="D34" s="45"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="45"/>
+      <c r="I34" s="45"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="45"/>
+      <c r="L34" s="45"/>
+      <c r="M34" s="45"/>
+      <c r="N34" s="45"/>
+      <c r="O34" s="45"/>
+      <c r="P34" s="45"/>
+      <c r="Q34" s="45"/>
+      <c r="R34" s="45"/>
+      <c r="S34" s="47"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B35" s="7" t="s">
@@ -3038,7 +3018,7 @@
       <c r="D35" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="65"/>
+      <c r="E35" s="79"/>
       <c r="F35" s="7" t="s">
         <v>72</v>
       </c>
@@ -3072,11 +3052,11 @@
       <c r="P35" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="Q35" s="60" t="s">
+      <c r="Q35" s="58" t="s">
         <v>163</v>
       </c>
-      <c r="R35" s="61"/>
-      <c r="S35" s="62"/>
+      <c r="R35" s="59"/>
+      <c r="S35" s="60"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B36" s="10" t="s">
@@ -3088,7 +3068,7 @@
       <c r="D36" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="66"/>
+      <c r="E36" s="80"/>
       <c r="F36" s="10"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -3102,15 +3082,15 @@
       <c r="N36" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="O36" s="44" t="s">
+      <c r="O36" s="61" t="s">
         <v>135</v>
       </c>
-      <c r="P36" s="71" t="s">
+      <c r="P36" s="85" t="s">
         <v>142</v>
       </c>
-      <c r="Q36" s="51"/>
-      <c r="R36" s="52"/>
-      <c r="S36" s="53"/>
+      <c r="Q36" s="49"/>
+      <c r="R36" s="50"/>
+      <c r="S36" s="51"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B37" s="10" t="s">
@@ -3122,7 +3102,7 @@
       <c r="D37" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="66"/>
+      <c r="E37" s="80"/>
       <c r="F37" s="10"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -3136,11 +3116,11 @@
       <c r="N37" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="O37" s="44"/>
-      <c r="P37" s="71"/>
-      <c r="Q37" s="54"/>
-      <c r="R37" s="55"/>
-      <c r="S37" s="56"/>
+      <c r="O37" s="61"/>
+      <c r="P37" s="85"/>
+      <c r="Q37" s="52"/>
+      <c r="R37" s="53"/>
+      <c r="S37" s="54"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B38" s="10" t="s">
@@ -3150,7 +3130,7 @@
       <c r="D38" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E38" s="66"/>
+      <c r="E38" s="80"/>
       <c r="F38" s="10"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -3164,11 +3144,11 @@
       <c r="N38" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="O38" s="44"/>
-      <c r="P38" s="71"/>
-      <c r="Q38" s="54"/>
-      <c r="R38" s="55"/>
-      <c r="S38" s="56"/>
+      <c r="O38" s="61"/>
+      <c r="P38" s="85"/>
+      <c r="Q38" s="52"/>
+      <c r="R38" s="53"/>
+      <c r="S38" s="54"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B39" s="10" t="s">
@@ -3178,7 +3158,7 @@
       <c r="D39" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="66"/>
+      <c r="E39" s="80"/>
       <c r="F39" s="10"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -3192,11 +3172,11 @@
       <c r="N39" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="O39" s="44"/>
-      <c r="P39" s="71"/>
-      <c r="Q39" s="54"/>
-      <c r="R39" s="55"/>
-      <c r="S39" s="56"/>
+      <c r="O39" s="61"/>
+      <c r="P39" s="85"/>
+      <c r="Q39" s="52"/>
+      <c r="R39" s="53"/>
+      <c r="S39" s="54"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B40" s="10" t="s">
@@ -3206,7 +3186,7 @@
       <c r="D40" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E40" s="66"/>
+      <c r="E40" s="80"/>
       <c r="F40" s="10"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -3220,11 +3200,11 @@
       <c r="N40" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="O40" s="44"/>
-      <c r="P40" s="71"/>
-      <c r="Q40" s="54"/>
-      <c r="R40" s="55"/>
-      <c r="S40" s="56"/>
+      <c r="O40" s="61"/>
+      <c r="P40" s="85"/>
+      <c r="Q40" s="52"/>
+      <c r="R40" s="53"/>
+      <c r="S40" s="54"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B41" s="10" t="s">
@@ -3234,7 +3214,7 @@
       <c r="D41" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E41" s="66"/>
+      <c r="E41" s="80"/>
       <c r="F41" s="10"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -3248,21 +3228,21 @@
       <c r="N41" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="O41" s="44"/>
-      <c r="P41" s="71"/>
-      <c r="Q41" s="54"/>
-      <c r="R41" s="55"/>
-      <c r="S41" s="56"/>
+      <c r="O41" s="61"/>
+      <c r="P41" s="85"/>
+      <c r="Q41" s="52"/>
+      <c r="R41" s="53"/>
+      <c r="S41" s="54"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B42" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C42" s="43"/>
+      <c r="C42" s="76"/>
       <c r="D42" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E42" s="66"/>
+      <c r="E42" s="80"/>
       <c r="F42" s="10"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -3276,11 +3256,11 @@
       <c r="N42" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="O42" s="44"/>
-      <c r="P42" s="71"/>
-      <c r="Q42" s="54"/>
-      <c r="R42" s="55"/>
-      <c r="S42" s="56"/>
+      <c r="O42" s="61"/>
+      <c r="P42" s="85"/>
+      <c r="Q42" s="52"/>
+      <c r="R42" s="53"/>
+      <c r="S42" s="54"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B43" s="10" t="s">
@@ -3292,7 +3272,7 @@
       <c r="D43" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E43" s="66"/>
+      <c r="E43" s="80"/>
       <c r="F43" s="10"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -3306,11 +3286,11 @@
       <c r="N43" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="O43" s="44"/>
-      <c r="P43" s="71"/>
-      <c r="Q43" s="54"/>
-      <c r="R43" s="55"/>
-      <c r="S43" s="56"/>
+      <c r="O43" s="61"/>
+      <c r="P43" s="85"/>
+      <c r="Q43" s="52"/>
+      <c r="R43" s="53"/>
+      <c r="S43" s="54"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B44" s="10" t="s">
@@ -3322,7 +3302,7 @@
       <c r="D44" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E44" s="66"/>
+      <c r="E44" s="80"/>
       <c r="F44" s="10"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -3336,23 +3316,23 @@
       <c r="N44" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="O44" s="44"/>
-      <c r="P44" s="71"/>
-      <c r="Q44" s="54"/>
-      <c r="R44" s="55"/>
-      <c r="S44" s="56"/>
+      <c r="O44" s="61"/>
+      <c r="P44" s="85"/>
+      <c r="Q44" s="52"/>
+      <c r="R44" s="53"/>
+      <c r="S44" s="54"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B45" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C45" s="44" t="s">
+      <c r="C45" s="61" t="s">
         <v>126</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E45" s="66"/>
+      <c r="E45" s="80"/>
       <c r="F45" s="10"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -3366,21 +3346,21 @@
       <c r="N45" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="O45" s="44"/>
-      <c r="P45" s="71"/>
-      <c r="Q45" s="54"/>
-      <c r="R45" s="55"/>
-      <c r="S45" s="56"/>
+      <c r="O45" s="61"/>
+      <c r="P45" s="85"/>
+      <c r="Q45" s="52"/>
+      <c r="R45" s="53"/>
+      <c r="S45" s="54"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B46" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="44"/>
+      <c r="C46" s="61"/>
       <c r="D46" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E46" s="66"/>
+      <c r="E46" s="80"/>
       <c r="F46" s="10"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
@@ -3394,11 +3374,11 @@
       <c r="N46" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="O46" s="44"/>
-      <c r="P46" s="71"/>
-      <c r="Q46" s="54"/>
-      <c r="R46" s="55"/>
-      <c r="S46" s="56"/>
+      <c r="O46" s="61"/>
+      <c r="P46" s="85"/>
+      <c r="Q46" s="52"/>
+      <c r="R46" s="53"/>
+      <c r="S46" s="54"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B47" s="10" t="s">
@@ -3410,7 +3390,7 @@
       <c r="D47" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="E47" s="66"/>
+      <c r="E47" s="80"/>
       <c r="F47" s="10"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -3424,11 +3404,11 @@
       <c r="N47" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="O47" s="44"/>
-      <c r="P47" s="71"/>
-      <c r="Q47" s="54"/>
-      <c r="R47" s="55"/>
-      <c r="S47" s="56"/>
+      <c r="O47" s="61"/>
+      <c r="P47" s="85"/>
+      <c r="Q47" s="52"/>
+      <c r="R47" s="53"/>
+      <c r="S47" s="54"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B48" s="10" t="s">
@@ -3438,7 +3418,7 @@
       <c r="D48" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="E48" s="66"/>
+      <c r="E48" s="80"/>
       <c r="F48" s="10"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -3452,11 +3432,11 @@
       <c r="N48" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="O48" s="44"/>
-      <c r="P48" s="71"/>
-      <c r="Q48" s="54"/>
-      <c r="R48" s="55"/>
-      <c r="S48" s="56"/>
+      <c r="O48" s="61"/>
+      <c r="P48" s="85"/>
+      <c r="Q48" s="52"/>
+      <c r="R48" s="53"/>
+      <c r="S48" s="54"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B49" s="10" t="s">
@@ -3464,7 +3444,7 @@
       </c>
       <c r="C49" s="42"/>
       <c r="D49" s="11"/>
-      <c r="E49" s="66"/>
+      <c r="E49" s="80"/>
       <c r="F49" s="10"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -3478,19 +3458,19 @@
       <c r="N49" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="O49" s="44"/>
-      <c r="P49" s="71"/>
-      <c r="Q49" s="54"/>
-      <c r="R49" s="55"/>
-      <c r="S49" s="56"/>
+      <c r="O49" s="61"/>
+      <c r="P49" s="85"/>
+      <c r="Q49" s="52"/>
+      <c r="R49" s="53"/>
+      <c r="S49" s="54"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B50" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="43"/>
+      <c r="C50" s="76"/>
       <c r="D50" s="11"/>
-      <c r="E50" s="66"/>
+      <c r="E50" s="80"/>
       <c r="F50" s="10"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -3501,22 +3481,22 @@
         <v>53</v>
       </c>
       <c r="M50" s="11"/>
-      <c r="N50" s="63" t="s">
+      <c r="N50" s="77" t="s">
         <v>105</v>
       </c>
-      <c r="O50" s="44" t="s">
+      <c r="O50" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="P50" s="71"/>
-      <c r="Q50" s="54"/>
-      <c r="R50" s="55"/>
-      <c r="S50" s="56"/>
+      <c r="P50" s="85"/>
+      <c r="Q50" s="52"/>
+      <c r="R50" s="53"/>
+      <c r="S50" s="54"/>
     </row>
     <row r="51" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B51" s="13"/>
       <c r="C51" s="24"/>
       <c r="D51" s="15"/>
-      <c r="E51" s="67"/>
+      <c r="E51" s="81"/>
       <c r="F51" s="13"/>
       <c r="G51" s="14"/>
       <c r="H51" s="14"/>
@@ -3527,18 +3507,20 @@
         <v>54</v>
       </c>
       <c r="M51" s="15"/>
-      <c r="N51" s="64"/>
-      <c r="O51" s="70"/>
-      <c r="P51" s="72"/>
-      <c r="Q51" s="57"/>
-      <c r="R51" s="58"/>
-      <c r="S51" s="59"/>
+      <c r="N51" s="78"/>
+      <c r="O51" s="84"/>
+      <c r="P51" s="86"/>
+      <c r="Q51" s="55"/>
+      <c r="R51" s="56"/>
+      <c r="S51" s="57"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.15">
       <c r="N52" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="C24:C26"/>
     <mergeCell ref="Q36:S51"/>
     <mergeCell ref="Q35:S35"/>
     <mergeCell ref="Q19:S19"/>
@@ -3553,6 +3535,8 @@
     <mergeCell ref="E19:E32"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="O29:O32"/>
     <mergeCell ref="C18:S18"/>
     <mergeCell ref="C2:S2"/>
     <mergeCell ref="C34:S34"/>
@@ -3567,11 +3551,7 @@
     <mergeCell ref="E3:E16"/>
     <mergeCell ref="O4:O11"/>
     <mergeCell ref="P4:P16"/>
-    <mergeCell ref="C37:C42"/>
     <mergeCell ref="C21:C23"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="O29:O32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
bikeride-lagom-20 Biker: Separate the behavior initial and postAdded
</commit_message>
<xml_diff>
--- a/doc/BikeRide-Model.xlsx
+++ b/doc/BikeRide-Model.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="204">
   <si>
     <t>Biker</t>
   </si>
@@ -1294,6 +1294,87 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1309,45 +1390,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1372,15 +1414,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1388,39 +1421,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1822,8 +1822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26:G30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20:N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.15"/>
@@ -1852,25 +1852,25 @@
       <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="75" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="47"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="M2" s="73"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="72"/>
+      <c r="P2" s="72"/>
+      <c r="Q2" s="72"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="74"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B3" s="7" t="s">
@@ -1882,7 +1882,7 @@
       <c r="D3" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="70"/>
+      <c r="E3" s="68"/>
       <c r="F3" s="7" t="s">
         <v>72</v>
       </c>
@@ -1916,11 +1916,11 @@
       <c r="P3" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="Q3" s="58" t="s">
+      <c r="Q3" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="R3" s="59"/>
-      <c r="S3" s="60"/>
+      <c r="R3" s="55"/>
+      <c r="S3" s="56"/>
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B4" s="10" t="s">
@@ -1932,7 +1932,7 @@
       <c r="D4" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="71"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="10" t="s">
         <v>74</v>
       </c>
@@ -1956,27 +1956,27 @@
       <c r="N4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="61" t="s">
+      <c r="O4" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="P4" s="73" t="s">
+      <c r="P4" s="84" t="s">
         <v>106</v>
       </c>
-      <c r="Q4" s="49"/>
-      <c r="R4" s="50"/>
-      <c r="S4" s="51"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="47"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B5" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="64" t="s">
         <v>90</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E5" s="71"/>
+      <c r="E5" s="69"/>
       <c r="F5" s="10" t="s">
         <v>76</v>
       </c>
@@ -2002,21 +2002,21 @@
       <c r="N5" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="73"/>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="53"/>
-      <c r="S5" s="54"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="50"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B6" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="C6" s="61"/>
+      <c r="C6" s="64"/>
       <c r="D6" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E6" s="71"/>
+      <c r="E6" s="69"/>
       <c r="F6" s="10" t="s">
         <v>76</v>
       </c>
@@ -2042,21 +2042,21 @@
       <c r="N6" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="O6" s="61"/>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="53"/>
-      <c r="S6" s="54"/>
+      <c r="O6" s="64"/>
+      <c r="P6" s="84"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="49"/>
+      <c r="S6" s="50"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B7" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C7" s="61"/>
+      <c r="C7" s="64"/>
       <c r="D7" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E7" s="71"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="10" t="s">
         <v>76</v>
       </c>
@@ -2082,21 +2082,21 @@
       <c r="N7" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="O7" s="61"/>
-      <c r="P7" s="73"/>
-      <c r="Q7" s="52"/>
-      <c r="R7" s="53"/>
-      <c r="S7" s="54"/>
+      <c r="O7" s="64"/>
+      <c r="P7" s="84"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="49"/>
+      <c r="S7" s="50"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B8" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="C8" s="61"/>
+      <c r="C8" s="64"/>
       <c r="D8" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E8" s="71"/>
+      <c r="E8" s="69"/>
       <c r="F8" s="10" t="s">
         <v>76</v>
       </c>
@@ -2122,21 +2122,21 @@
       <c r="N8" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="O8" s="61"/>
-      <c r="P8" s="73"/>
-      <c r="Q8" s="52"/>
-      <c r="R8" s="53"/>
-      <c r="S8" s="54"/>
+      <c r="O8" s="64"/>
+      <c r="P8" s="84"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="50"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B9" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="C9" s="61"/>
+      <c r="C9" s="64"/>
       <c r="D9" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="71"/>
+      <c r="E9" s="69"/>
       <c r="F9" s="10" t="s">
         <v>76</v>
       </c>
@@ -2162,21 +2162,21 @@
       <c r="N9" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="O9" s="61"/>
-      <c r="P9" s="73"/>
-      <c r="Q9" s="52"/>
-      <c r="R9" s="53"/>
-      <c r="S9" s="54"/>
+      <c r="O9" s="64"/>
+      <c r="P9" s="84"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="49"/>
+      <c r="S9" s="50"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B10" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C10" s="61"/>
+      <c r="C10" s="64"/>
       <c r="D10" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="71"/>
+      <c r="E10" s="69"/>
       <c r="F10" s="10" t="s">
         <v>74</v>
       </c>
@@ -2200,17 +2200,17 @@
       <c r="N10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="O10" s="61"/>
-      <c r="P10" s="73"/>
-      <c r="Q10" s="52"/>
-      <c r="R10" s="53"/>
-      <c r="S10" s="54"/>
+      <c r="O10" s="64"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="49"/>
+      <c r="S10" s="50"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B11" s="10"/>
-      <c r="C11" s="62"/>
+      <c r="C11" s="76"/>
       <c r="D11" s="11"/>
-      <c r="E11" s="71"/>
+      <c r="E11" s="69"/>
       <c r="F11" s="10" t="s">
         <v>74</v>
       </c>
@@ -2234,17 +2234,17 @@
       <c r="N11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="O11" s="61"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="52"/>
-      <c r="R11" s="53"/>
-      <c r="S11" s="54"/>
+      <c r="O11" s="64"/>
+      <c r="P11" s="84"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="49"/>
+      <c r="S11" s="50"/>
     </row>
     <row r="12" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B12" s="10"/>
-      <c r="C12" s="62"/>
+      <c r="C12" s="76"/>
       <c r="D12" s="11"/>
-      <c r="E12" s="71"/>
+      <c r="E12" s="69"/>
       <c r="F12" s="10" t="s">
         <v>85</v>
       </c>
@@ -2265,26 +2265,26 @@
         <v>194</v>
       </c>
       <c r="M12" s="11"/>
-      <c r="N12" s="65"/>
-      <c r="O12" s="63" t="s">
+      <c r="N12" s="79"/>
+      <c r="O12" s="77" t="s">
         <v>136</v>
       </c>
-      <c r="P12" s="73"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="54"/>
+      <c r="P12" s="84"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="49"/>
+      <c r="S12" s="50"/>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B13" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C13" s="63" t="s">
+      <c r="C13" s="77" t="s">
         <v>156</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E13" s="71"/>
+      <c r="E13" s="69"/>
       <c r="F13" s="10" t="s">
         <v>85</v>
       </c>
@@ -2305,22 +2305,22 @@
         <v>198</v>
       </c>
       <c r="M13" s="11"/>
-      <c r="N13" s="66"/>
-      <c r="O13" s="68"/>
-      <c r="P13" s="73"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="53"/>
-      <c r="S13" s="54"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="82"/>
+      <c r="P13" s="84"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="49"/>
+      <c r="S13" s="50"/>
     </row>
     <row r="14" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B14" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="C14" s="64"/>
+      <c r="C14" s="78"/>
       <c r="D14" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="E14" s="71"/>
+      <c r="E14" s="69"/>
       <c r="F14" s="10" t="s">
         <v>85</v>
       </c>
@@ -2340,19 +2340,21 @@
       <c r="L14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="11"/>
-      <c r="N14" s="66"/>
-      <c r="O14" s="68"/>
-      <c r="P14" s="73"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="53"/>
-      <c r="S14" s="54"/>
+      <c r="M14" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="N14" s="80"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="84"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="49"/>
+      <c r="S14" s="50"/>
     </row>
     <row r="15" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B15" s="39"/>
       <c r="C15" s="29"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="71"/>
+      <c r="E15" s="69"/>
       <c r="F15" s="10" t="s">
         <v>85</v>
       </c>
@@ -2373,18 +2375,18 @@
         <v>13</v>
       </c>
       <c r="M15" s="11"/>
-      <c r="N15" s="66"/>
-      <c r="O15" s="68"/>
-      <c r="P15" s="74"/>
-      <c r="Q15" s="52"/>
-      <c r="R15" s="53"/>
-      <c r="S15" s="54"/>
+      <c r="N15" s="80"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="85"/>
+      <c r="Q15" s="48"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="50"/>
     </row>
     <row r="16" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="13"/>
       <c r="C16" s="24"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="72"/>
+      <c r="E16" s="70"/>
       <c r="F16" s="13" t="s">
         <v>85</v>
       </c>
@@ -2405,12 +2407,12 @@
         <v>202</v>
       </c>
       <c r="M16" s="15"/>
-      <c r="N16" s="67"/>
-      <c r="O16" s="69"/>
-      <c r="P16" s="75"/>
-      <c r="Q16" s="55"/>
-      <c r="R16" s="56"/>
-      <c r="S16" s="57"/>
+      <c r="N16" s="81"/>
+      <c r="O16" s="83"/>
+      <c r="P16" s="86"/>
+      <c r="Q16" s="51"/>
+      <c r="R16" s="52"/>
+      <c r="S16" s="53"/>
     </row>
     <row r="17" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="P17" s="16"/>
@@ -2419,25 +2421,25 @@
       <c r="B18" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="44" t="s">
+      <c r="C18" s="71" t="s">
         <v>187</v>
       </c>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="46"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="45"/>
-      <c r="S18" s="47"/>
+      <c r="D18" s="72"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+      <c r="H18" s="72"/>
+      <c r="I18" s="72"/>
+      <c r="J18" s="72"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="72"/>
+      <c r="O18" s="72"/>
+      <c r="P18" s="72"/>
+      <c r="Q18" s="72"/>
+      <c r="R18" s="72"/>
+      <c r="S18" s="74"/>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B19" s="7" t="s">
@@ -2449,7 +2451,7 @@
       <c r="D19" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="70"/>
+      <c r="E19" s="68"/>
       <c r="F19" s="7" t="s">
         <v>72</v>
       </c>
@@ -2483,11 +2485,11 @@
       <c r="P19" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="Q19" s="58" t="s">
+      <c r="Q19" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="R19" s="59"/>
-      <c r="S19" s="60"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="56"/>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B20" s="10" t="s">
@@ -2499,7 +2501,7 @@
       <c r="D20" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="71"/>
+      <c r="E20" s="69"/>
       <c r="F20" s="10" t="s">
         <v>74</v>
       </c>
@@ -2523,27 +2525,27 @@
       <c r="N20" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O20" s="61" t="s">
+      <c r="O20" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="P20" s="82" t="s">
+      <c r="P20" s="62" t="s">
         <v>188</v>
       </c>
-      <c r="Q20" s="49"/>
-      <c r="R20" s="50"/>
-      <c r="S20" s="51"/>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="46"/>
+      <c r="S20" s="47"/>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B21" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="C21" s="61" t="s">
+      <c r="C21" s="64" t="s">
         <v>131</v>
       </c>
       <c r="D21" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E21" s="71"/>
+      <c r="E21" s="69"/>
       <c r="F21" s="10" t="s">
         <v>76</v>
       </c>
@@ -2569,21 +2571,21 @@
       <c r="N21" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="O21" s="61"/>
-      <c r="P21" s="82"/>
-      <c r="Q21" s="52"/>
-      <c r="R21" s="53"/>
-      <c r="S21" s="54"/>
+      <c r="O21" s="64"/>
+      <c r="P21" s="62"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="49"/>
+      <c r="S21" s="50"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B22" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="C22" s="61"/>
+      <c r="C22" s="64"/>
       <c r="D22" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E22" s="71"/>
+      <c r="E22" s="69"/>
       <c r="F22" s="10" t="s">
         <v>76</v>
       </c>
@@ -2609,21 +2611,21 @@
       <c r="N22" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="O22" s="61"/>
-      <c r="P22" s="82"/>
-      <c r="Q22" s="52"/>
-      <c r="R22" s="53"/>
-      <c r="S22" s="54"/>
+      <c r="O22" s="64"/>
+      <c r="P22" s="62"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="49"/>
+      <c r="S22" s="50"/>
     </row>
     <row r="23" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B23" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="C23" s="61"/>
+      <c r="C23" s="64"/>
       <c r="D23" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="E23" s="71"/>
+      <c r="E23" s="69"/>
       <c r="F23" s="10" t="s">
         <v>74</v>
       </c>
@@ -2647,11 +2649,11 @@
       <c r="N23" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="O23" s="61"/>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="52"/>
-      <c r="R23" s="53"/>
-      <c r="S23" s="54"/>
+      <c r="O23" s="64"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="49"/>
+      <c r="S23" s="50"/>
     </row>
     <row r="24" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B24" s="10" t="s">
@@ -2663,7 +2665,7 @@
       <c r="D24" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="71"/>
+      <c r="E24" s="69"/>
       <c r="F24" s="10" t="s">
         <v>74</v>
       </c>
@@ -2687,11 +2689,11 @@
       <c r="N24" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="O24" s="61"/>
-      <c r="P24" s="82"/>
-      <c r="Q24" s="52"/>
-      <c r="R24" s="53"/>
-      <c r="S24" s="54"/>
+      <c r="O24" s="64"/>
+      <c r="P24" s="62"/>
+      <c r="Q24" s="48"/>
+      <c r="R24" s="49"/>
+      <c r="S24" s="50"/>
     </row>
     <row r="25" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B25" s="10" t="s">
@@ -2701,7 +2703,7 @@
       <c r="D25" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="71"/>
+      <c r="E25" s="69"/>
       <c r="F25" s="10" t="s">
         <v>74</v>
       </c>
@@ -2727,21 +2729,21 @@
       <c r="N25" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O25" s="61"/>
-      <c r="P25" s="82"/>
-      <c r="Q25" s="52"/>
-      <c r="R25" s="53"/>
-      <c r="S25" s="54"/>
+      <c r="O25" s="64"/>
+      <c r="P25" s="62"/>
+      <c r="Q25" s="48"/>
+      <c r="R25" s="49"/>
+      <c r="S25" s="50"/>
     </row>
     <row r="26" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B26" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="C26" s="76"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="71"/>
+      <c r="E26" s="69"/>
       <c r="F26" s="10" t="s">
         <v>173</v>
       </c>
@@ -2765,17 +2767,17 @@
       <c r="N26" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="O26" s="61"/>
-      <c r="P26" s="82"/>
-      <c r="Q26" s="52"/>
-      <c r="R26" s="53"/>
-      <c r="S26" s="54"/>
+      <c r="O26" s="64"/>
+      <c r="P26" s="62"/>
+      <c r="Q26" s="48"/>
+      <c r="R26" s="49"/>
+      <c r="S26" s="50"/>
     </row>
     <row r="27" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B27" s="10"/>
-      <c r="C27" s="61"/>
+      <c r="C27" s="64"/>
       <c r="D27" s="11"/>
-      <c r="E27" s="71"/>
+      <c r="E27" s="69"/>
       <c r="F27" s="10" t="s">
         <v>74</v>
       </c>
@@ -2799,17 +2801,17 @@
       <c r="N27" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="O27" s="61"/>
-      <c r="P27" s="82"/>
-      <c r="Q27" s="52"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="54"/>
+      <c r="O27" s="64"/>
+      <c r="P27" s="62"/>
+      <c r="Q27" s="48"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="50"/>
     </row>
     <row r="28" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B28" s="10"/>
-      <c r="C28" s="61"/>
+      <c r="C28" s="64"/>
       <c r="D28" s="11"/>
-      <c r="E28" s="71"/>
+      <c r="E28" s="69"/>
       <c r="F28" s="31" t="s">
         <v>74</v>
       </c>
@@ -2833,17 +2835,17 @@
       <c r="N28" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="O28" s="61"/>
-      <c r="P28" s="82"/>
-      <c r="Q28" s="52"/>
-      <c r="R28" s="53"/>
-      <c r="S28" s="54"/>
+      <c r="O28" s="64"/>
+      <c r="P28" s="62"/>
+      <c r="Q28" s="48"/>
+      <c r="R28" s="49"/>
+      <c r="S28" s="50"/>
     </row>
     <row r="29" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B29" s="10"/>
       <c r="C29" s="30"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="71"/>
+      <c r="E29" s="69"/>
       <c r="F29" s="10" t="s">
         <v>85</v>
       </c>
@@ -2868,10 +2870,10 @@
       <c r="O29" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="P29" s="82"/>
-      <c r="Q29" s="52"/>
-      <c r="R29" s="53"/>
-      <c r="S29" s="54"/>
+      <c r="P29" s="62"/>
+      <c r="Q29" s="48"/>
+      <c r="R29" s="49"/>
+      <c r="S29" s="50"/>
     </row>
     <row r="30" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B30" s="10" t="s">
@@ -2883,7 +2885,7 @@
       <c r="D30" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E30" s="71"/>
+      <c r="E30" s="69"/>
       <c r="F30" s="10" t="s">
         <v>85</v>
       </c>
@@ -2906,10 +2908,10 @@
       <c r="M30" s="11"/>
       <c r="N30" s="25"/>
       <c r="O30" s="42"/>
-      <c r="P30" s="82"/>
-      <c r="Q30" s="52"/>
-      <c r="R30" s="53"/>
-      <c r="S30" s="54"/>
+      <c r="P30" s="62"/>
+      <c r="Q30" s="48"/>
+      <c r="R30" s="49"/>
+      <c r="S30" s="50"/>
     </row>
     <row r="31" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B31" s="10" t="s">
@@ -2919,7 +2921,7 @@
       <c r="D31" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E31" s="71"/>
+      <c r="E31" s="69"/>
       <c r="F31" s="10" t="s">
         <v>85</v>
       </c>
@@ -2942,10 +2944,10 @@
       <c r="M31" s="11"/>
       <c r="N31" s="25"/>
       <c r="O31" s="42"/>
-      <c r="P31" s="82"/>
-      <c r="Q31" s="52"/>
-      <c r="R31" s="53"/>
-      <c r="S31" s="54"/>
+      <c r="P31" s="62"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="49"/>
+      <c r="S31" s="50"/>
     </row>
     <row r="32" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B32" s="13" t="s">
@@ -2955,7 +2957,7 @@
       <c r="D32" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="E32" s="72"/>
+      <c r="E32" s="70"/>
       <c r="F32" s="13" t="s">
         <v>85</v>
       </c>
@@ -2978,35 +2980,35 @@
       <c r="M32" s="15"/>
       <c r="N32" s="38"/>
       <c r="O32" s="43"/>
-      <c r="P32" s="83"/>
-      <c r="Q32" s="55"/>
-      <c r="R32" s="56"/>
-      <c r="S32" s="57"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="51"/>
+      <c r="R32" s="52"/>
+      <c r="S32" s="53"/>
     </row>
     <row r="33" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="34" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B34" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="44" t="s">
+      <c r="C34" s="71" t="s">
         <v>124</v>
       </c>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="45"/>
-      <c r="J34" s="45"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="45"/>
-      <c r="M34" s="45"/>
-      <c r="N34" s="45"/>
-      <c r="O34" s="45"/>
-      <c r="P34" s="45"/>
-      <c r="Q34" s="45"/>
-      <c r="R34" s="45"/>
-      <c r="S34" s="47"/>
+      <c r="D34" s="72"/>
+      <c r="E34" s="72"/>
+      <c r="F34" s="72"/>
+      <c r="G34" s="72"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="72"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="72"/>
+      <c r="M34" s="72"/>
+      <c r="N34" s="72"/>
+      <c r="O34" s="72"/>
+      <c r="P34" s="72"/>
+      <c r="Q34" s="72"/>
+      <c r="R34" s="72"/>
+      <c r="S34" s="74"/>
     </row>
     <row r="35" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B35" s="7" t="s">
@@ -3018,7 +3020,7 @@
       <c r="D35" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E35" s="79"/>
+      <c r="E35" s="59"/>
       <c r="F35" s="7" t="s">
         <v>72</v>
       </c>
@@ -3052,11 +3054,11 @@
       <c r="P35" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="Q35" s="58" t="s">
+      <c r="Q35" s="54" t="s">
         <v>163</v>
       </c>
-      <c r="R35" s="59"/>
-      <c r="S35" s="60"/>
+      <c r="R35" s="55"/>
+      <c r="S35" s="56"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B36" s="10" t="s">
@@ -3068,7 +3070,7 @@
       <c r="D36" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="80"/>
+      <c r="E36" s="60"/>
       <c r="F36" s="10"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -3082,15 +3084,15 @@
       <c r="N36" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="O36" s="61" t="s">
+      <c r="O36" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="P36" s="85" t="s">
+      <c r="P36" s="66" t="s">
         <v>142</v>
       </c>
-      <c r="Q36" s="49"/>
-      <c r="R36" s="50"/>
-      <c r="S36" s="51"/>
+      <c r="Q36" s="45"/>
+      <c r="R36" s="46"/>
+      <c r="S36" s="47"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B37" s="10" t="s">
@@ -3102,7 +3104,7 @@
       <c r="D37" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="80"/>
+      <c r="E37" s="60"/>
       <c r="F37" s="10"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -3116,11 +3118,11 @@
       <c r="N37" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="O37" s="61"/>
-      <c r="P37" s="85"/>
-      <c r="Q37" s="52"/>
-      <c r="R37" s="53"/>
-      <c r="S37" s="54"/>
+      <c r="O37" s="64"/>
+      <c r="P37" s="66"/>
+      <c r="Q37" s="48"/>
+      <c r="R37" s="49"/>
+      <c r="S37" s="50"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B38" s="10" t="s">
@@ -3130,7 +3132,7 @@
       <c r="D38" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E38" s="80"/>
+      <c r="E38" s="60"/>
       <c r="F38" s="10"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -3144,11 +3146,11 @@
       <c r="N38" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="O38" s="61"/>
-      <c r="P38" s="85"/>
-      <c r="Q38" s="52"/>
-      <c r="R38" s="53"/>
-      <c r="S38" s="54"/>
+      <c r="O38" s="64"/>
+      <c r="P38" s="66"/>
+      <c r="Q38" s="48"/>
+      <c r="R38" s="49"/>
+      <c r="S38" s="50"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B39" s="10" t="s">
@@ -3158,7 +3160,7 @@
       <c r="D39" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="80"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="10"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -3172,11 +3174,11 @@
       <c r="N39" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="O39" s="61"/>
-      <c r="P39" s="85"/>
-      <c r="Q39" s="52"/>
-      <c r="R39" s="53"/>
-      <c r="S39" s="54"/>
+      <c r="O39" s="64"/>
+      <c r="P39" s="66"/>
+      <c r="Q39" s="48"/>
+      <c r="R39" s="49"/>
+      <c r="S39" s="50"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B40" s="10" t="s">
@@ -3186,7 +3188,7 @@
       <c r="D40" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="E40" s="80"/>
+      <c r="E40" s="60"/>
       <c r="F40" s="10"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -3200,11 +3202,11 @@
       <c r="N40" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="O40" s="61"/>
-      <c r="P40" s="85"/>
-      <c r="Q40" s="52"/>
-      <c r="R40" s="53"/>
-      <c r="S40" s="54"/>
+      <c r="O40" s="64"/>
+      <c r="P40" s="66"/>
+      <c r="Q40" s="48"/>
+      <c r="R40" s="49"/>
+      <c r="S40" s="50"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B41" s="10" t="s">
@@ -3214,7 +3216,7 @@
       <c r="D41" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E41" s="80"/>
+      <c r="E41" s="60"/>
       <c r="F41" s="10"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -3228,21 +3230,21 @@
       <c r="N41" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="O41" s="61"/>
-      <c r="P41" s="85"/>
-      <c r="Q41" s="52"/>
-      <c r="R41" s="53"/>
-      <c r="S41" s="54"/>
+      <c r="O41" s="64"/>
+      <c r="P41" s="66"/>
+      <c r="Q41" s="48"/>
+      <c r="R41" s="49"/>
+      <c r="S41" s="50"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B42" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C42" s="76"/>
+      <c r="C42" s="44"/>
       <c r="D42" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E42" s="80"/>
+      <c r="E42" s="60"/>
       <c r="F42" s="10"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -3256,11 +3258,11 @@
       <c r="N42" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="O42" s="61"/>
-      <c r="P42" s="85"/>
-      <c r="Q42" s="52"/>
-      <c r="R42" s="53"/>
-      <c r="S42" s="54"/>
+      <c r="O42" s="64"/>
+      <c r="P42" s="66"/>
+      <c r="Q42" s="48"/>
+      <c r="R42" s="49"/>
+      <c r="S42" s="50"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B43" s="10" t="s">
@@ -3272,7 +3274,7 @@
       <c r="D43" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E43" s="80"/>
+      <c r="E43" s="60"/>
       <c r="F43" s="10"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -3286,11 +3288,11 @@
       <c r="N43" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="O43" s="61"/>
-      <c r="P43" s="85"/>
-      <c r="Q43" s="52"/>
-      <c r="R43" s="53"/>
-      <c r="S43" s="54"/>
+      <c r="O43" s="64"/>
+      <c r="P43" s="66"/>
+      <c r="Q43" s="48"/>
+      <c r="R43" s="49"/>
+      <c r="S43" s="50"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B44" s="10" t="s">
@@ -3302,7 +3304,7 @@
       <c r="D44" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="E44" s="80"/>
+      <c r="E44" s="60"/>
       <c r="F44" s="10"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -3316,23 +3318,23 @@
       <c r="N44" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="O44" s="61"/>
-      <c r="P44" s="85"/>
-      <c r="Q44" s="52"/>
-      <c r="R44" s="53"/>
-      <c r="S44" s="54"/>
+      <c r="O44" s="64"/>
+      <c r="P44" s="66"/>
+      <c r="Q44" s="48"/>
+      <c r="R44" s="49"/>
+      <c r="S44" s="50"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B45" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C45" s="61" t="s">
+      <c r="C45" s="64" t="s">
         <v>126</v>
       </c>
       <c r="D45" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E45" s="80"/>
+      <c r="E45" s="60"/>
       <c r="F45" s="10"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -3346,21 +3348,21 @@
       <c r="N45" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="O45" s="61"/>
-      <c r="P45" s="85"/>
-      <c r="Q45" s="52"/>
-      <c r="R45" s="53"/>
-      <c r="S45" s="54"/>
+      <c r="O45" s="64"/>
+      <c r="P45" s="66"/>
+      <c r="Q45" s="48"/>
+      <c r="R45" s="49"/>
+      <c r="S45" s="50"/>
     </row>
     <row r="46" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B46" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="C46" s="61"/>
+      <c r="C46" s="64"/>
       <c r="D46" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="E46" s="80"/>
+      <c r="E46" s="60"/>
       <c r="F46" s="10"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
@@ -3374,11 +3376,11 @@
       <c r="N46" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="O46" s="61"/>
-      <c r="P46" s="85"/>
-      <c r="Q46" s="52"/>
-      <c r="R46" s="53"/>
-      <c r="S46" s="54"/>
+      <c r="O46" s="64"/>
+      <c r="P46" s="66"/>
+      <c r="Q46" s="48"/>
+      <c r="R46" s="49"/>
+      <c r="S46" s="50"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B47" s="10" t="s">
@@ -3390,7 +3392,7 @@
       <c r="D47" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="E47" s="80"/>
+      <c r="E47" s="60"/>
       <c r="F47" s="10"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -3404,11 +3406,11 @@
       <c r="N47" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="O47" s="61"/>
-      <c r="P47" s="85"/>
-      <c r="Q47" s="52"/>
-      <c r="R47" s="53"/>
-      <c r="S47" s="54"/>
+      <c r="O47" s="64"/>
+      <c r="P47" s="66"/>
+      <c r="Q47" s="48"/>
+      <c r="R47" s="49"/>
+      <c r="S47" s="50"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B48" s="10" t="s">
@@ -3418,7 +3420,7 @@
       <c r="D48" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="E48" s="80"/>
+      <c r="E48" s="60"/>
       <c r="F48" s="10"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -3432,11 +3434,11 @@
       <c r="N48" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="O48" s="61"/>
-      <c r="P48" s="85"/>
-      <c r="Q48" s="52"/>
-      <c r="R48" s="53"/>
-      <c r="S48" s="54"/>
+      <c r="O48" s="64"/>
+      <c r="P48" s="66"/>
+      <c r="Q48" s="48"/>
+      <c r="R48" s="49"/>
+      <c r="S48" s="50"/>
     </row>
     <row r="49" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B49" s="10" t="s">
@@ -3444,7 +3446,7 @@
       </c>
       <c r="C49" s="42"/>
       <c r="D49" s="11"/>
-      <c r="E49" s="80"/>
+      <c r="E49" s="60"/>
       <c r="F49" s="10"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -3458,19 +3460,19 @@
       <c r="N49" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="O49" s="61"/>
-      <c r="P49" s="85"/>
-      <c r="Q49" s="52"/>
-      <c r="R49" s="53"/>
-      <c r="S49" s="54"/>
+      <c r="O49" s="64"/>
+      <c r="P49" s="66"/>
+      <c r="Q49" s="48"/>
+      <c r="R49" s="49"/>
+      <c r="S49" s="50"/>
     </row>
     <row r="50" spans="2:19" x14ac:dyDescent="0.15">
       <c r="B50" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="76"/>
+      <c r="C50" s="44"/>
       <c r="D50" s="11"/>
-      <c r="E50" s="80"/>
+      <c r="E50" s="60"/>
       <c r="F50" s="10"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -3481,22 +3483,22 @@
         <v>53</v>
       </c>
       <c r="M50" s="11"/>
-      <c r="N50" s="77" t="s">
+      <c r="N50" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="O50" s="61" t="s">
+      <c r="O50" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="P50" s="85"/>
-      <c r="Q50" s="52"/>
-      <c r="R50" s="53"/>
-      <c r="S50" s="54"/>
+      <c r="P50" s="66"/>
+      <c r="Q50" s="48"/>
+      <c r="R50" s="49"/>
+      <c r="S50" s="50"/>
     </row>
     <row r="51" spans="2:19" ht="12" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B51" s="13"/>
       <c r="C51" s="24"/>
       <c r="D51" s="15"/>
-      <c r="E51" s="81"/>
+      <c r="E51" s="61"/>
       <c r="F51" s="13"/>
       <c r="G51" s="14"/>
       <c r="H51" s="14"/>
@@ -3507,18 +3509,35 @@
         <v>54</v>
       </c>
       <c r="M51" s="15"/>
-      <c r="N51" s="78"/>
-      <c r="O51" s="84"/>
-      <c r="P51" s="86"/>
-      <c r="Q51" s="55"/>
-      <c r="R51" s="56"/>
-      <c r="S51" s="57"/>
+      <c r="N51" s="58"/>
+      <c r="O51" s="65"/>
+      <c r="P51" s="67"/>
+      <c r="Q51" s="51"/>
+      <c r="R51" s="52"/>
+      <c r="S51" s="53"/>
     </row>
     <row r="52" spans="2:19" x14ac:dyDescent="0.15">
       <c r="N52" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C37:C42"/>
+    <mergeCell ref="O29:O32"/>
+    <mergeCell ref="C18:S18"/>
+    <mergeCell ref="C2:S2"/>
+    <mergeCell ref="C34:S34"/>
+    <mergeCell ref="Q4:S16"/>
+    <mergeCell ref="Q20:S32"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="C5:C10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="N12:N16"/>
+    <mergeCell ref="O12:O16"/>
+    <mergeCell ref="E3:E16"/>
+    <mergeCell ref="O4:O11"/>
+    <mergeCell ref="P4:P16"/>
     <mergeCell ref="C30:C32"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="Q36:S51"/>
@@ -3535,23 +3554,6 @@
     <mergeCell ref="E19:E32"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C37:C42"/>
-    <mergeCell ref="O29:O32"/>
-    <mergeCell ref="C18:S18"/>
-    <mergeCell ref="C2:S2"/>
-    <mergeCell ref="C34:S34"/>
-    <mergeCell ref="Q4:S16"/>
-    <mergeCell ref="Q20:S32"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="C5:C10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="N12:N16"/>
-    <mergeCell ref="O12:O16"/>
-    <mergeCell ref="E3:E16"/>
-    <mergeCell ref="O4:O11"/>
-    <mergeCell ref="P4:P16"/>
-    <mergeCell ref="C21:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>